<commit_message>
Subiendo actualizacion planilla cliente.xlsx
</commit_message>
<xml_diff>
--- a/config/clientes.xlsx
+++ b/config/clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">servicio</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Oficina Copiapo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365652-7</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -187,8 +190,8 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>365652</v>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>